<commit_message>
Addition of extractable cations
</commit_message>
<xml_diff>
--- a/data/processed/CN.xlsx
+++ b/data/processed/CN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/penninoa/Documents/VT/Data/MyData/Soil_Analyses/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADA05C3-C22D-014B-B634-643D05957051}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCBCBFA-C869-7748-BCD1-8D97F7121192}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31700" yWindow="3760" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="195">
   <si>
     <t>CNRatio</t>
   </si>
@@ -538,9 +538,6 @@
     <t>D5</t>
   </si>
   <si>
-    <t>D11</t>
-  </si>
-  <si>
     <t>52_4_d2</t>
   </si>
   <si>
@@ -602,6 +599,12 @@
   </si>
   <si>
     <t>86_2_W2.2</t>
+  </si>
+  <si>
+    <t>BC3</t>
+  </si>
+  <si>
+    <t>D10</t>
   </si>
 </sst>
 </file>
@@ -1110,8 +1113,8 @@
   </sheetPr>
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E154" sqref="E154"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="K132" sqref="K132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1121,28 +1124,28 @@
   <sheetData>
     <row r="1" spans="1:20" s="50" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="49" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>183</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
@@ -1406,7 +1409,7 @@
     </row>
     <row r="10" spans="1:20" ht="15.75" customHeight="1">
       <c r="A10" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>10</v>
@@ -1435,7 +1438,7 @@
     </row>
     <row r="11" spans="1:20" ht="15.75" customHeight="1">
       <c r="A11" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>11</v>
@@ -1464,7 +1467,7 @@
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1">
       <c r="A12" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>12</v>
@@ -1493,7 +1496,7 @@
     </row>
     <row r="13" spans="1:20" ht="15.75" customHeight="1">
       <c r="A13" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>13</v>
@@ -1522,7 +1525,7 @@
     </row>
     <row r="14" spans="1:20" ht="15.75" customHeight="1">
       <c r="A14" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>14</v>
@@ -1551,7 +1554,7 @@
     </row>
     <row r="15" spans="1:20" ht="15.75" customHeight="1">
       <c r="A15" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>15</v>
@@ -1580,7 +1583,7 @@
     </row>
     <row r="16" spans="1:20" ht="15.75" customHeight="1">
       <c r="A16" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>16</v>
@@ -1609,7 +1612,7 @@
     </row>
     <row r="17" spans="1:20" ht="15.75" customHeight="1">
       <c r="A17" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>17</v>
@@ -1638,7 +1641,7 @@
     </row>
     <row r="18" spans="1:20" ht="15.75" customHeight="1">
       <c r="A18" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>18</v>
@@ -1667,7 +1670,7 @@
     </row>
     <row r="19" spans="1:20" ht="15.75" customHeight="1">
       <c r="A19" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>19</v>
@@ -1696,7 +1699,7 @@
     </row>
     <row r="20" spans="1:20" ht="15.75" customHeight="1">
       <c r="A20" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>20</v>
@@ -1725,7 +1728,7 @@
     </row>
     <row r="21" spans="1:20" ht="15.75" customHeight="1">
       <c r="A21" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>21</v>
@@ -1754,7 +1757,7 @@
     </row>
     <row r="22" spans="1:20" ht="15.75" customHeight="1">
       <c r="A22" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>22</v>
@@ -1783,7 +1786,7 @@
     </row>
     <row r="23" spans="1:20" ht="15.75" customHeight="1">
       <c r="A23" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>23</v>
@@ -1812,7 +1815,7 @@
     </row>
     <row r="24" spans="1:20" ht="15.75" customHeight="1">
       <c r="A24" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>24</v>
@@ -1841,7 +1844,7 @@
     </row>
     <row r="25" spans="1:20" ht="15.75" customHeight="1">
       <c r="A25" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>25</v>
@@ -1870,7 +1873,7 @@
     </row>
     <row r="26" spans="1:20" ht="15.75" customHeight="1">
       <c r="A26" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>26</v>
@@ -1899,7 +1902,7 @@
     </row>
     <row r="27" spans="1:20" ht="15.75" customHeight="1">
       <c r="A27" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>27</v>
@@ -1928,7 +1931,7 @@
     </row>
     <row r="28" spans="1:20" ht="15.75" customHeight="1">
       <c r="A28" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>28</v>
@@ -1989,7 +1992,7 @@
     </row>
     <row r="30" spans="1:20" ht="15.75" customHeight="1">
       <c r="A30" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>29</v>
@@ -2018,7 +2021,7 @@
     </row>
     <row r="31" spans="1:20" ht="15.75" customHeight="1">
       <c r="A31" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>30</v>
@@ -2047,7 +2050,7 @@
     </row>
     <row r="32" spans="1:20" ht="15.75" customHeight="1">
       <c r="A32" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>31</v>
@@ -2076,7 +2079,7 @@
     </row>
     <row r="33" spans="1:20" ht="15.75" customHeight="1">
       <c r="A33" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>32</v>
@@ -2105,7 +2108,7 @@
     </row>
     <row r="34" spans="1:20" ht="15.75" customHeight="1">
       <c r="A34" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>33</v>
@@ -2134,7 +2137,7 @@
     </row>
     <row r="35" spans="1:20" ht="15.75" customHeight="1">
       <c r="A35" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>34</v>
@@ -2163,7 +2166,7 @@
     </row>
     <row r="36" spans="1:20" ht="15.75" customHeight="1">
       <c r="A36" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>35</v>
@@ -2192,7 +2195,7 @@
     </row>
     <row r="37" spans="1:20" ht="15.75" customHeight="1">
       <c r="A37" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>36</v>
@@ -2221,7 +2224,7 @@
     </row>
     <row r="38" spans="1:20" ht="15.75" customHeight="1">
       <c r="A38" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>37</v>
@@ -2250,7 +2253,7 @@
     </row>
     <row r="39" spans="1:20" ht="15.75" customHeight="1">
       <c r="A39" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>38</v>
@@ -2279,7 +2282,7 @@
     </row>
     <row r="40" spans="1:20" ht="15.75" customHeight="1">
       <c r="A40" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>39</v>
@@ -2308,7 +2311,7 @@
     </row>
     <row r="41" spans="1:20" ht="15.75" customHeight="1">
       <c r="A41" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>40</v>
@@ -2473,7 +2476,7 @@
     </row>
     <row r="46" spans="1:20" ht="15.75" customHeight="1">
       <c r="A46" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>45</v>
@@ -2502,7 +2505,7 @@
     </row>
     <row r="47" spans="1:20" ht="15.75" customHeight="1">
       <c r="A47" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>46</v>
@@ -2531,7 +2534,7 @@
     </row>
     <row r="48" spans="1:20" ht="13">
       <c r="A48" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>47</v>
@@ -2560,7 +2563,7 @@
     </row>
     <row r="49" spans="1:20" ht="13">
       <c r="A49" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>48</v>
@@ -2621,7 +2624,7 @@
     </row>
     <row r="51" spans="1:20" ht="13">
       <c r="A51" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>49</v>
@@ -2650,7 +2653,7 @@
     </row>
     <row r="52" spans="1:20" ht="13">
       <c r="A52" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>50</v>
@@ -2679,7 +2682,7 @@
     </row>
     <row r="53" spans="1:20" ht="13">
       <c r="A53" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>51</v>
@@ -2708,7 +2711,7 @@
     </row>
     <row r="54" spans="1:20" ht="13">
       <c r="A54" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>52</v>
@@ -2737,7 +2740,7 @@
     </row>
     <row r="55" spans="1:20" ht="13">
       <c r="A55" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>53</v>
@@ -2766,7 +2769,7 @@
     </row>
     <row r="56" spans="1:20" ht="13">
       <c r="A56" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>54</v>
@@ -2795,7 +2798,7 @@
     </row>
     <row r="57" spans="1:20" ht="13">
       <c r="A57" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>55</v>
@@ -2824,7 +2827,7 @@
     </row>
     <row r="58" spans="1:20" ht="14">
       <c r="A58" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>56</v>
@@ -2853,7 +2856,7 @@
     </row>
     <row r="59" spans="1:20" ht="14">
       <c r="A59" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>57</v>
@@ -2882,7 +2885,7 @@
     </row>
     <row r="60" spans="1:20" ht="14">
       <c r="A60" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>58</v>
@@ -2911,7 +2914,7 @@
     </row>
     <row r="61" spans="1:20" ht="14">
       <c r="A61" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>59</v>
@@ -2940,7 +2943,7 @@
     </row>
     <row r="62" spans="1:20" ht="13">
       <c r="A62" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>60</v>
@@ -2978,7 +2981,7 @@
     </row>
     <row r="63" spans="1:20" ht="13">
       <c r="A63" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>61</v>
@@ -3007,7 +3010,7 @@
     </row>
     <row r="64" spans="1:20" ht="13">
       <c r="A64" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>62</v>
@@ -3045,7 +3048,7 @@
     </row>
     <row r="65" spans="1:20" ht="13">
       <c r="A65" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>63</v>
@@ -3074,7 +3077,7 @@
     </row>
     <row r="66" spans="1:20" ht="13">
       <c r="A66" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>64</v>
@@ -3103,13 +3106,13 @@
     </row>
     <row r="67" spans="1:20" ht="14">
       <c r="A67" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C67" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D67" s="16" t="s">
         <v>123</v>
@@ -3132,16 +3135,16 @@
     </row>
     <row r="68" spans="1:20" ht="14">
       <c r="A68" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C68" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E68" s="35">
         <v>0.512992</v>
@@ -3161,13 +3164,13 @@
     </row>
     <row r="69" spans="1:20" ht="14">
       <c r="A69" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C69" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D69" s="29" t="s">
         <v>125</v>
@@ -3190,13 +3193,13 @@
     </row>
     <row r="70" spans="1:20" ht="14">
       <c r="A70" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C70" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D70" s="16" t="s">
         <v>144</v>
@@ -3251,13 +3254,13 @@
     </row>
     <row r="72" spans="1:20" ht="14">
       <c r="A72" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C72" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D72" s="16" t="s">
         <v>145</v>
@@ -3280,13 +3283,13 @@
     </row>
     <row r="73" spans="1:20" ht="14">
       <c r="A73" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C73" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D73" s="16" t="s">
         <v>168</v>
@@ -3309,13 +3312,13 @@
     </row>
     <row r="74" spans="1:20" ht="14">
       <c r="A74" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B74" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C74" s="29" t="s">
         <v>191</v>
-      </c>
-      <c r="C74" s="29" t="s">
-        <v>192</v>
       </c>
       <c r="D74" s="16" t="s">
         <v>169</v>
@@ -3338,7 +3341,7 @@
     </row>
     <row r="75" spans="1:20" ht="13">
       <c r="A75" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>65</v>
@@ -3367,7 +3370,7 @@
     </row>
     <row r="76" spans="1:20" ht="13">
       <c r="A76" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>66</v>
@@ -3396,7 +3399,7 @@
     </row>
     <row r="77" spans="1:20" ht="13">
       <c r="A77" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>67</v>
@@ -3425,7 +3428,7 @@
     </row>
     <row r="78" spans="1:20" ht="13">
       <c r="A78" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>68</v>
@@ -3454,7 +3457,7 @@
     </row>
     <row r="79" spans="1:20" ht="13">
       <c r="A79" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>69</v>
@@ -3483,7 +3486,7 @@
     </row>
     <row r="80" spans="1:20" ht="13">
       <c r="A80" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>70</v>
@@ -3512,7 +3515,7 @@
     </row>
     <row r="81" spans="1:20" ht="13">
       <c r="A81" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>71</v>
@@ -3541,7 +3544,7 @@
     </row>
     <row r="82" spans="1:20" ht="13">
       <c r="A82" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>72</v>
@@ -3570,7 +3573,7 @@
     </row>
     <row r="83" spans="1:20" ht="13">
       <c r="A83" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>73</v>
@@ -3599,7 +3602,7 @@
     </row>
     <row r="84" spans="1:20" ht="13">
       <c r="A84" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>74</v>
@@ -3628,7 +3631,7 @@
     </row>
     <row r="85" spans="1:20" ht="13">
       <c r="A85" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>75</v>
@@ -3657,7 +3660,7 @@
     </row>
     <row r="86" spans="1:20" ht="13">
       <c r="A86" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>76</v>
@@ -3686,7 +3689,7 @@
     </row>
     <row r="87" spans="1:20" ht="13">
       <c r="A87" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>77</v>
@@ -3715,7 +3718,7 @@
     </row>
     <row r="88" spans="1:20" ht="13">
       <c r="A88" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>78</v>
@@ -3744,7 +3747,7 @@
     </row>
     <row r="89" spans="1:20" ht="13">
       <c r="A89" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>79</v>
@@ -3773,7 +3776,7 @@
     </row>
     <row r="90" spans="1:20" ht="13">
       <c r="A90" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>80</v>
@@ -3802,7 +3805,7 @@
     </row>
     <row r="91" spans="1:20" ht="13">
       <c r="A91" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>81</v>
@@ -3863,7 +3866,7 @@
     </row>
     <row r="93" spans="1:20" ht="13">
       <c r="A93" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>82</v>
@@ -3892,7 +3895,7 @@
     </row>
     <row r="94" spans="1:20" ht="13">
       <c r="A94" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>83</v>
@@ -3901,7 +3904,7 @@
         <v>162</v>
       </c>
       <c r="D94" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E94" s="35">
         <v>1.2055E-2</v>
@@ -3921,7 +3924,7 @@
     </row>
     <row r="95" spans="1:20" ht="13">
       <c r="A95" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>84</v>
@@ -3950,7 +3953,7 @@
     </row>
     <row r="96" spans="1:20" ht="13">
       <c r="A96" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>85</v>
@@ -3979,7 +3982,7 @@
     </row>
     <row r="97" spans="1:20" ht="13">
       <c r="A97" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>86</v>
@@ -4008,7 +4011,7 @@
     </row>
     <row r="98" spans="1:20" ht="13">
       <c r="A98" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>87</v>
@@ -4037,7 +4040,7 @@
     </row>
     <row r="99" spans="1:20" ht="13">
       <c r="A99" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>88</v>
@@ -4066,7 +4069,7 @@
     </row>
     <row r="100" spans="1:20" ht="13">
       <c r="A100" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>89</v>
@@ -4095,7 +4098,7 @@
     </row>
     <row r="101" spans="1:20" ht="13">
       <c r="A101" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>90</v>
@@ -4124,7 +4127,7 @@
     </row>
     <row r="102" spans="1:20" ht="13">
       <c r="A102" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>91</v>
@@ -4619,13 +4622,13 @@
     </row>
     <row r="116" spans="1:20" ht="13">
       <c r="A116" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>105</v>
       </c>
       <c r="C116" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D116" s="16">
         <v>3</v>
@@ -4648,7 +4651,7 @@
     </row>
     <row r="117" spans="1:20" ht="13">
       <c r="A117" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>106</v>
@@ -4677,7 +4680,7 @@
     </row>
     <row r="118" spans="1:20" ht="13">
       <c r="A118" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>107</v>
@@ -4706,7 +4709,7 @@
     </row>
     <row r="119" spans="1:20" ht="13">
       <c r="A119" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>108</v>
@@ -4735,7 +4738,7 @@
     </row>
     <row r="120" spans="1:20" ht="13">
       <c r="A120" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>109</v>
@@ -4764,7 +4767,7 @@
     </row>
     <row r="121" spans="1:20" ht="13">
       <c r="A121" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>110</v>
@@ -4793,7 +4796,7 @@
     </row>
     <row r="122" spans="1:20" ht="13">
       <c r="A122" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>111</v>
@@ -4822,7 +4825,7 @@
     </row>
     <row r="123" spans="1:20" ht="13">
       <c r="A123" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>112</v>
@@ -4851,7 +4854,7 @@
     </row>
     <row r="124" spans="1:20" ht="13">
       <c r="A124" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B124" s="4" t="s">
         <v>113</v>
@@ -4880,7 +4883,7 @@
     </row>
     <row r="125" spans="1:20" ht="13">
       <c r="A125" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>114</v>
@@ -4909,7 +4912,7 @@
     </row>
     <row r="126" spans="1:20" ht="13">
       <c r="A126" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B126" s="4" t="s">
         <v>115</v>
@@ -4918,7 +4921,7 @@
         <v>167</v>
       </c>
       <c r="D126" s="24" t="s">
-        <v>150</v>
+        <v>193</v>
       </c>
       <c r="E126" s="35">
         <v>4.6387999999999999E-2</v>
@@ -4938,7 +4941,7 @@
     </row>
     <row r="127" spans="1:20" ht="13">
       <c r="A127" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>116</v>
@@ -4947,7 +4950,7 @@
         <v>167</v>
       </c>
       <c r="D127" s="24" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="E127" s="35">
         <v>1.2708000000000001E-2</v>
@@ -4967,7 +4970,7 @@
     </row>
     <row r="128" spans="1:20" ht="13">
       <c r="A128" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>117</v>
@@ -4976,7 +4979,7 @@
         <v>167</v>
       </c>
       <c r="D128" s="16" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="E128" s="35">
         <v>9.5700000000000004E-3</v>
@@ -5228,7 +5231,7 @@
     </row>
     <row r="136" spans="1:20" ht="13">
       <c r="A136" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>92</v>
@@ -5257,7 +5260,7 @@
     </row>
     <row r="137" spans="1:20" ht="13">
       <c r="A137" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>94</v>
@@ -5286,7 +5289,7 @@
     </row>
     <row r="138" spans="1:20" ht="13">
       <c r="A138" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>95</v>
@@ -5315,7 +5318,7 @@
     </row>
     <row r="139" spans="1:20" ht="13">
       <c r="A139" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>96</v>
@@ -5344,7 +5347,7 @@
     </row>
     <row r="140" spans="1:20" ht="13">
       <c r="A140" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>97</v>
@@ -5373,7 +5376,7 @@
     </row>
     <row r="141" spans="1:20" ht="13">
       <c r="A141" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B141" s="10" t="s">
         <v>98</v>
@@ -5411,7 +5414,7 @@
     </row>
     <row r="142" spans="1:20" ht="13">
       <c r="A142" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B142" s="10" t="s">
         <v>99</v>
@@ -5449,13 +5452,13 @@
     </row>
     <row r="143" spans="1:20" ht="14">
       <c r="A143" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B143" s="10" t="s">
         <v>100</v>
       </c>
       <c r="C143" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D143" s="29" t="s">
         <v>123</v>
@@ -5487,13 +5490,13 @@
     </row>
     <row r="144" spans="1:20" ht="14">
       <c r="A144" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B144" s="10" t="s">
         <v>101</v>
       </c>
       <c r="C144" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D144" s="29" t="s">
         <v>121</v>
@@ -5525,13 +5528,13 @@
     </row>
     <row r="145" spans="1:20" ht="14">
       <c r="A145" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B145" s="10" t="s">
         <v>102</v>
       </c>
       <c r="C145" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D145" s="28" t="s">
         <v>122</v>
@@ -5563,13 +5566,13 @@
     </row>
     <row r="146" spans="1:20" ht="13">
       <c r="A146" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B146" s="10" t="s">
         <v>103</v>
       </c>
       <c r="C146" s="28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D146" s="28">
         <v>2</v>
@@ -5601,13 +5604,13 @@
     </row>
     <row r="147" spans="1:20" ht="13">
       <c r="A147" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B147" s="10" t="s">
         <v>104</v>
       </c>
       <c r="C147" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D147" s="28">
         <v>2</v>

</xml_diff>